<commit_message>
Se ordena y se limpia la interfaz de usuario, se agrega funcion de editar TN
</commit_message>
<xml_diff>
--- a/atributos.xlsx
+++ b/atributos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,28 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tercer atributo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ojnfwjf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>owirjfw</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>iwejrgpwergf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregan iconos a botones, se agrega funcionalidad de edición en atributos, se agrega filtro por TN
</commit_message>
<xml_diff>
--- a/atributos.xlsx
+++ b/atributos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pjfwpejf</t>
+          <t>Una definición más propia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>iwjfwf</t>
+          <t>Una regla más propia</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>efweff</t>
+          <t>Palabra_1, Palabra_2</t>
         </is>
       </c>
     </row>
@@ -562,6 +562,72 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>iwejrgpwergf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Calle</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>iojfiwjfifj de la calle</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>iojargiwjfpowfdpo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>street, otro</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>calculo que seiuhnfowijef</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>varianza de cartera + varianza de clientes = bono</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>comisión, cantidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Escuela</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Definición de la escuela</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Se calculñaijw0ijfqwopkf</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>academia</t>
         </is>
       </c>
     </row>

</xml_diff>